<commit_message>
Review class Parameters and dataProvider
</commit_message>
<xml_diff>
--- a/testdata/Excel.xlsx
+++ b/testdata/Excel.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9CFFAC44-C177-4CAB-8993-ED6F5DBEF82D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE6764F-9A1E-4928-BB5D-E7F98A85D5DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="22350" windowHeight="13800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="Employee" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -399,7 +403,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +415,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -439,7 +443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>